<commit_message>
Updated README.MD and made other small changes
</commit_message>
<xml_diff>
--- a/data/tuckshop.xlsx
+++ b/data/tuckshop.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awhiskin/tuckshop/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awhiskin/eclipse-workspace/tuckshop/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
   <si>
     <t>Form</t>
   </si>
@@ -92,15 +92,6 @@
     <t>Anonymous</t>
   </si>
   <si>
-    <t>26/02/2017 | 14:25</t>
-  </si>
-  <si>
-    <t>197320016988:YJkKulTD</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>Kid</t>
   </si>
   <si>
@@ -111,24 +102,6 @@
   </si>
   <si>
     <t>Parent@example.com</t>
-  </si>
-  <si>
-    <t>White High Fibre Bread , Cheese, Chicken Breast - Sliced</t>
-  </si>
-  <si>
-    <t>Orange Juice, Apple Juice</t>
-  </si>
-  <si>
-    <t>Apple, Banana</t>
-  </si>
-  <si>
-    <t>Lemonade Ice Block, Fruit Cup (Stewed fruit natural juice)</t>
-  </si>
-  <si>
-    <t>Hot Dog without Sauce, Fresh Corn 1/2 Cob</t>
-  </si>
-  <si>
-    <t>Apple</t>
   </si>
   <si>
     <t>26/02/2017 | 15:08</t>
@@ -524,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A5" activeCellId="1" sqref="A2:XFD3 A5:XFD5"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,52 +569,58 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
       <c r="D2">
-        <v>1186076</v>
+        <v>1186084</v>
       </c>
       <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
       </c>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R2" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -649,58 +628,58 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="D3">
-        <v>1186084</v>
+        <v>1186085</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="S3" t="s">
         <v>36</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" t="s">
-        <v>40</v>
-      </c>
-      <c r="O3" t="s">
-        <v>41</v>
-      </c>
-      <c r="P3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>43</v>
-      </c>
-      <c r="R3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -708,58 +687,58 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="D4">
-        <v>1186085</v>
+        <v>1186086</v>
       </c>
       <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="S4" t="s">
         <v>39</v>
-      </c>
-      <c r="N4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>43</v>
-      </c>
-      <c r="R4" t="s">
-        <v>44</v>
-      </c>
-      <c r="S4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -767,108 +746,49 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5">
-        <v>1186086</v>
+        <v>1186172</v>
       </c>
       <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" t="s">
         <v>47</v>
       </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" t="s">
-        <v>38</v>
-      </c>
       <c r="M5" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="O5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="P5" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="R5" t="s">
-        <v>44</v>
-      </c>
-      <c r="S5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>1186172</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" t="s">
         <v>51</v>
-      </c>
-      <c r="G6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" t="s">
-        <v>56</v>
-      </c>
-      <c r="M6" t="s">
-        <v>57</v>
-      </c>
-      <c r="O6" t="s">
-        <v>58</v>
-      </c>
-      <c r="P6" t="s">
-        <v>59</v>
-      </c>
-      <c r="R6" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>